<commit_message>
PIN-847: improve handling unresolvable duplicities
</commit_message>
<xml_diff>
--- a/tests/NewApiBundle/Resources/KHM-Import-4HH-0HHM.xlsx
+++ b/tests/NewApiBundle/Resources/KHM-Import-4HH-0HHM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="152">
   <si>
     <t xml:space="preserve">Address street</t>
   </si>
@@ -613,8 +613,8 @@
   </sheetPr>
   <dimension ref="A1:BG10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL10" activeCellId="0" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1351,6 +1351,12 @@
       <c r="AF7" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="AK7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <v>132</v>
+      </c>
       <c r="BD7" s="6" t="s">
         <v>136</v>
       </c>
@@ -1398,6 +1404,12 @@
       <c r="AF8" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="AK8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <v>88</v>
+      </c>
       <c r="BD8" s="6" t="s">
         <v>136</v>
       </c>
@@ -1444,6 +1456,12 @@
       </c>
       <c r="AF9" s="3" t="s">
         <v>95</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL9" s="0" t="n">
+        <v>61561</v>
       </c>
       <c r="BD9" s="6" t="s">
         <v>136</v>

</xml_diff>